<commit_message>
LoadFlow supernode BuildMatrix bug fix
</commit_message>
<xml_diff>
--- a/Docs/Tanh PQ PV.xlsx
+++ b/Docs/Tanh PQ PV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masha\source\repos\DFW2\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA0FF9C-A6A1-443D-AE05-E3332D011221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1C3D96-00CB-4666-BCA5-6AD7EB7D3F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2655BF34-683B-45E4-95B3-B9559C8928E3}"/>
   </bookViews>
@@ -252,67 +252,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>299.99981645866387</c:v>
+                  <c:v>199.99932701695354</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>299.9991774256759</c:v>
+                  <c:v>199.99698393135904</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>299.99631349523867</c:v>
+                  <c:v>199.98648356330125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>299.98347858533123</c:v>
+                  <c:v>199.93943648847124</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>299.92596325440826</c:v>
+                  <c:v>199.72883307757701</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>299.66833281784579</c:v>
+                  <c:v>198.78990721970672</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>298.51642610601897</c:v>
+                  <c:v>194.67864833164086</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>293.40783442164314</c:v>
+                  <c:v>178.0037682405632</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>271.54447609345533</c:v>
+                  <c:v>126.87516245373516</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>190.54468571616903</c:v>
+                  <c:v>48.084019114437915</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-190.5446857161881</c:v>
+                  <c:v>-15.198277390225371</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-271.54447609346107</c:v>
+                  <c:v>-18.91011073504184</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-293.40783442164451</c:v>
+                  <c:v>-19.755873276451368</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-298.51642610601925</c:v>
+                  <c:v>-19.945480966030772</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-299.66833281784591</c:v>
+                  <c:v>-19.987832816804655</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-299.92596325440826</c:v>
+                  <c:v>-19.997285017815642</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-299.98347858533123</c:v>
+                  <c:v>-19.999394199782486</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-299.99631349523867</c:v>
+                  <c:v>-19.999864827411272</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-299.9991774256759</c:v>
+                  <c:v>-19.999969838904235</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-299.99981645866387</c:v>
+                  <c:v>-19.999993270149133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="E1">
         <f>TANH($B$4*($B$1-D1-$B$7))*$B$5+$B$6</f>
-        <v>299.99981645866387</v>
+        <v>199.99932701695354</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>-300</v>
+        <v>-20</v>
       </c>
       <c r="D2">
         <f>D1+($D$11-$D$1)/10</f>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E21" si="0">TANH($B$4*($B$1-D2-$B$7))*$B$5+$B$6</f>
-        <v>299.9991774256759</v>
+        <v>199.99698393135904</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1450,7 +1450,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D10" si="1">D2+($D$11-$D$1)/10</f>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>299.99631349523867</v>
+        <v>199.98648356330125</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>299.98347858533123</v>
+        <v>199.93943648847124</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B5" s="1">
         <f>(B3-B2)/2</f>
-        <v>300</v>
+        <v>110</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>299.92596325440826</v>
+        <v>199.72883307757701</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="B6" s="1">
         <f>(B2+B3)/2</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>299.66833281784579</v>
+        <v>198.78990721970672</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1516,7 +1516,8 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <f>ATANH(B6/B5)/B4</f>
+        <v>7.6752836433134866E-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
@@ -1524,7 +1525,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>298.51642610601897</v>
+        <v>194.67864833164086</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1534,7 +1535,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>293.40783442164314</v>
+        <v>178.0037682405632</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1544,7 +1545,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>271.54447609345533</v>
+        <v>126.87516245373516</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1554,7 +1555,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>190.54468571616903</v>
+        <v>48.084019114437915</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1573,7 +1574,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>-190.5446857161881</v>
+        <v>-15.198277390225371</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,7 +1584,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>-271.54447609346107</v>
+        <v>-18.91011073504184</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1593,7 +1594,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>-293.40783442164451</v>
+        <v>-19.755873276451368</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,7 +1604,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>-298.51642610601925</v>
+        <v>-19.945480966030772</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,7 +1614,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>-299.66833281784591</v>
+        <v>-19.987832816804655</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
@@ -1623,7 +1624,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>-299.92596325440826</v>
+        <v>-19.997285017815642</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
@@ -1633,7 +1634,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-299.98347858533123</v>
+        <v>-19.999394199782486</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
@@ -1643,7 +1644,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-299.99631349523867</v>
+        <v>-19.999864827411272</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
@@ -1653,7 +1654,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>-299.9991774256759</v>
+        <v>-19.999969838904235</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
@@ -1663,7 +1664,7 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>-299.99981645866387</v>
+        <v>-19.999993270149133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LoadFlow tang centering (not working though)
</commit_message>
<xml_diff>
--- a/Docs/Tanh PQ PV.xlsx
+++ b/Docs/Tanh PQ PV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masha\source\repos\DFW2\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1C3D96-00CB-4666-BCA5-6AD7EB7D3F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F5298A-884E-4D2A-9A9D-F244232891A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2655BF34-683B-45E4-95B3-B9559C8928E3}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Vref</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Beta</t>
+  </si>
+  <si>
+    <t>VrQ</t>
+  </si>
+  <si>
+    <t>Kg</t>
   </si>
 </sst>
 </file>
@@ -252,67 +258,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>199.99932701695354</c:v>
+                  <c:v>199.99999999999227</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>199.99698393135904</c:v>
+                  <c:v>199.999999998855</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>199.98648356330125</c:v>
+                  <c:v>199.9999998300658</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>199.93943648847124</c:v>
+                  <c:v>199.9999747795361</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>199.72883307757701</c:v>
+                  <c:v>199.99625702085922</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>198.78990721970672</c:v>
+                  <c:v>199.4460209707365</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>194.67864833164086</c:v>
+                  <c:v>141.61991838098726</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>178.0037682405632</c:v>
+                  <c:v>3.2164443074122744</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>126.87516245373516</c:v>
+                  <c:v>2.2024040212215823E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48.084019114437915</c:v>
+                  <c:v>1.4841304883361772E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>9.9999998326438799E-7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.7379488655205932E-9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5403680815070402E-11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8421709430404007E-13</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>-15.198277390225371</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-18.91011073504184</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-19.755873276451368</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-19.945480966030772</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>-19.987832816804655</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-19.997285017815642</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-19.999394199782486</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-19.999864827411272</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-19.999969838904235</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-19.999993270149133</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1409,7 +1415,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1432,7 @@
       </c>
       <c r="E1">
         <f>TANH($B$4*($B$1-D1-$B$7))*$B$5+$B$6</f>
-        <v>199.99932701695354</v>
+        <v>199.99999999999227</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,7 +1440,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>-20</v>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>B2*(1-B9)</f>
+        <v>0</v>
       </c>
       <c r="D2">
         <f>D1+($D$11-$D$1)/10</f>
@@ -1442,7 +1452,7 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E21" si="0">TANH($B$4*($B$1-D2-$B$7))*$B$5+$B$6</f>
-        <v>199.99698393135904</v>
+        <v>199.999999998855</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1452,13 +1462,17 @@
       <c r="B3" s="1">
         <v>200</v>
       </c>
+      <c r="C3">
+        <f>B3*(1-B9)</f>
+        <v>199.99979999999999</v>
+      </c>
       <c r="D3">
         <f t="shared" ref="D3:D10" si="1">D2+($D$11-$D$1)/10</f>
         <v>10.100000000000001</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>199.98648356330125</v>
+        <v>199.9999998300658</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1466,7 +1480,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
@@ -1474,7 +1488,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>199.93943648847124</v>
+        <v>199.9999747795361</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,7 +1497,7 @@
       </c>
       <c r="B5" s="1">
         <f>(B3-B2)/2</f>
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
@@ -1491,7 +1505,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>199.72883307757701</v>
+        <v>199.99625702085922</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,7 +1514,7 @@
       </c>
       <c r="B6" s="1">
         <f>(B2+B3)/2</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
@@ -1508,7 +1522,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>198.78990721970672</v>
+        <v>199.4460209707365</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1516,8 +1530,8 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <f>ATANH(B6/B5)/B4</f>
-        <v>7.6752836433134866E-2</v>
+        <f>-ATANH((B8-B6)/B5)/B4</f>
+        <v>0.19113827925589782</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
@@ -1525,37 +1539,54 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>194.67864833164086</v>
+        <v>141.61991838098726</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>MIN(B3 - B9,MAX(0,B2 + B9))</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="D8">
         <f t="shared" si="1"/>
         <v>10.350000000000005</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>178.0037682405632</v>
+        <v>3.2164443074122744</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="D9">
         <f t="shared" si="1"/>
         <v>10.400000000000006</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>126.87516245373516</v>
+        <v>2.2024040212215823E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>(B8-B6)/B5</f>
+        <v>-0.99999999000000006</v>
+      </c>
       <c r="D10">
         <f t="shared" si="1"/>
         <v>10.450000000000006</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>48.084019114437915</v>
+        <v>1.4841304883361772E-4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,7 +1595,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.9999998326438799E-7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1574,7 +1605,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>-15.198277390225371</v>
+        <v>6.7379488655205932E-9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1584,7 +1615,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>-18.91011073504184</v>
+        <v>4.5403680815070402E-11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1594,7 +1625,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>-19.755873276451368</v>
+        <v>2.8421709430404007E-13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1604,7 +1635,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>-19.945480966030772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1614,7 +1645,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>-19.987832816804655</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
@@ -1624,7 +1655,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>-19.997285017815642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
@@ -1634,7 +1665,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-19.999394199782486</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
@@ -1644,7 +1675,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-19.999864827411272</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
@@ -1654,7 +1685,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>-19.999969838904235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
@@ -1664,7 +1695,7 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>-19.999993270149133</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>